<commit_message>
Add all data to exports
</commit_message>
<xml_diff>
--- a/assets/template.xlsx
+++ b/assets/template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Main\Workspace\NVNA-Schedule-Exporter\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Main\Workspace\NVNA-Schedule-Exporter\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95CA315B-F676-41C2-9994-0407C01464AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD5ED4E-371C-44DF-9D4F-40EF5BC92E84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="61">
   <si>
     <t>УТВЪРЖДАВАМ:</t>
   </si>
@@ -318,12 +318,6 @@
       </rPr>
       <t xml:space="preserve"> на обучение</t>
     </r>
-  </si>
-  <si>
-    <t>62221102</t>
-  </si>
-  <si>
-    <t>20000</t>
   </si>
 </sst>
 </file>
@@ -1035,7 +1029,7 @@
   <dimension ref="A1:AQ402"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="Q89" sqref="Q89"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1692,30 +1686,16 @@
       <c r="AQ12" s="1"/>
     </row>
     <row r="13" spans="1:43" ht="14" x14ac:dyDescent="0.3">
-      <c r="A13" s="50" t="s">
-        <v>62</v>
-      </c>
-      <c r="B13" s="51">
-        <v>100001</v>
-      </c>
-      <c r="C13" s="51">
-        <v>40</v>
-      </c>
-      <c r="D13" s="26">
-        <v>15</v>
-      </c>
-      <c r="E13" s="24">
-        <v>1</v>
-      </c>
-      <c r="F13" s="24">
-        <v>20</v>
-      </c>
-      <c r="G13" s="24">
-        <v>20</v>
-      </c>
+      <c r="A13" s="50"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
       <c r="H13" s="25">
         <f t="shared" ref="H13:H26" si="0">((IF(C13&lt;100,IF(C13&lt;10,0.1*C13*D13*2,D13*2),D13*3)+G13*(IF(F13&lt;=10,0.1*F13,1))))</f>
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="I13" s="26"/>
       <c r="J13" s="26"/>
@@ -1736,7 +1716,7 @@
       </c>
       <c r="W13" s="25">
         <f t="shared" ref="W13:W26" si="2">SUM(H13+V13)</f>
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="X13" s="27"/>
       <c r="Y13" s="28"/>
@@ -2542,7 +2522,10 @@
       <c r="E28" s="55"/>
       <c r="F28" s="51"/>
       <c r="G28" s="53"/>
-      <c r="H28" s="25"/>
+      <c r="H28" s="41">
+        <f t="shared" ref="H28" si="3">((IF(C28&lt;100,D28*2,D28*3)))+G28</f>
+        <v>0</v>
+      </c>
       <c r="I28" s="24"/>
       <c r="J28" s="24"/>
       <c r="K28" s="24"/>
@@ -2588,7 +2571,7 @@
       <c r="F29" s="24"/>
       <c r="G29" s="31"/>
       <c r="H29" s="25">
-        <f t="shared" ref="H29:H30" si="3">((IF(C29&lt;100,D29*2,D29*3)))+G29</f>
+        <f t="shared" ref="H29:H30" si="4">((IF(C29&lt;100,D29*2,D29*3)))+G29</f>
         <v>0</v>
       </c>
       <c r="I29" s="24"/>
@@ -2605,11 +2588,11 @@
       <c r="T29" s="24"/>
       <c r="U29" s="24"/>
       <c r="V29" s="25">
-        <f t="shared" ref="V29:V30" si="4">(I29*0.25)+(J29*0.15)+(K29*0.1)+(L29*0.1)+(M29*0.3)+(N29*4)+(O29*4)+(IF((P29*15)&gt;40,40,(P29*15)))+(IF((Q29*2)&gt;16,16,(Q29*2)))+(R29*120)+(S29*60)+(IF((T29*3)&gt;15,15,(T29*3))+(IF((U29*6)&gt;60,60,(U29*6))))</f>
+        <f t="shared" ref="V29:V30" si="5">(I29*0.25)+(J29*0.15)+(K29*0.1)+(L29*0.1)+(M29*0.3)+(N29*4)+(O29*4)+(IF((P29*15)&gt;40,40,(P29*15)))+(IF((Q29*2)&gt;16,16,(Q29*2)))+(R29*120)+(S29*60)+(IF((T29*3)&gt;15,15,(T29*3))+(IF((U29*6)&gt;60,60,(U29*6))))</f>
         <v>0</v>
       </c>
       <c r="W29" s="25">
-        <f t="shared" ref="W29:W30" si="5">SUM(H29+V29)</f>
+        <f t="shared" ref="W29:W30" si="6">SUM(H29+V29)</f>
         <v>0</v>
       </c>
       <c r="X29" s="28"/>
@@ -2642,7 +2625,7 @@
       <c r="F30" s="24"/>
       <c r="G30" s="31"/>
       <c r="H30" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I30" s="24"/>
@@ -2659,11 +2642,11 @@
       <c r="T30" s="24"/>
       <c r="U30" s="24"/>
       <c r="V30" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="W30" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="X30" s="28"/>
@@ -2769,7 +2752,7 @@
       <c r="F32" s="24"/>
       <c r="G32" s="31"/>
       <c r="H32" s="25">
-        <f t="shared" ref="H32:H36" si="6">(((IF(C32&lt;100,D32*2,D32*3)))+G32)*1.5</f>
+        <f t="shared" ref="H32:H36" si="7">(((IF(C32&lt;100,D32*2,D32*3)))+G32)*1.5</f>
         <v>0</v>
       </c>
       <c r="I32" s="24"/>
@@ -2786,11 +2769,11 @@
       <c r="T32" s="24"/>
       <c r="U32" s="24"/>
       <c r="V32" s="25">
-        <f t="shared" ref="V32:V36" si="7">(I32*0.25)+(J32*0.15)+(K32*0.1)+(L32*0.1)+(M32*0.3)+(N32*4)+(O32*4)+(IF((P32*15)&gt;40,40,(P32*15)))+(IF((Q32*2)&gt;16,16,(Q32*2)))+(R32*120)+(S32*60)+(IF((T32*3)&gt;15,15,(T32*3))+(IF((U32*6)&gt;60,60,(U32*6))))</f>
+        <f t="shared" ref="V32:V36" si="8">(I32*0.25)+(J32*0.15)+(K32*0.1)+(L32*0.1)+(M32*0.3)+(N32*4)+(O32*4)+(IF((P32*15)&gt;40,40,(P32*15)))+(IF((Q32*2)&gt;16,16,(Q32*2)))+(R32*120)+(S32*60)+(IF((T32*3)&gt;15,15,(T32*3))+(IF((U32*6)&gt;60,60,(U32*6))))</f>
         <v>0</v>
       </c>
       <c r="W32" s="25">
-        <f t="shared" ref="W32:W36" si="8">SUM(H32+V32)</f>
+        <f t="shared" ref="W32:W36" si="9">SUM(H32+V32)</f>
         <v>0</v>
       </c>
       <c r="X32" s="32"/>
@@ -2823,7 +2806,7 @@
       <c r="F33" s="24"/>
       <c r="G33" s="30"/>
       <c r="H33" s="25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I33" s="24"/>
@@ -2840,11 +2823,11 @@
       <c r="T33" s="24"/>
       <c r="U33" s="24"/>
       <c r="V33" s="25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W33" s="25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X33" s="32"/>
@@ -2877,7 +2860,7 @@
       <c r="F34" s="24"/>
       <c r="G34" s="31"/>
       <c r="H34" s="25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I34" s="24"/>
@@ -2894,11 +2877,11 @@
       <c r="T34" s="24"/>
       <c r="U34" s="24"/>
       <c r="V34" s="25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W34" s="25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X34" s="28"/>
@@ -2931,7 +2914,7 @@
       <c r="F35" s="24"/>
       <c r="G35" s="31"/>
       <c r="H35" s="25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I35" s="24"/>
@@ -2948,11 +2931,11 @@
       <c r="T35" s="24"/>
       <c r="U35" s="24"/>
       <c r="V35" s="25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W35" s="25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X35" s="28"/>
@@ -2985,7 +2968,7 @@
       <c r="F36" s="24"/>
       <c r="G36" s="31"/>
       <c r="H36" s="25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I36" s="24"/>
@@ -3002,11 +2985,11 @@
       <c r="T36" s="24"/>
       <c r="U36" s="24"/>
       <c r="V36" s="25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W36" s="25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X36" s="28"/>
@@ -3167,7 +3150,7 @@
       <c r="F39" s="62"/>
       <c r="G39" s="61"/>
       <c r="H39" s="25">
-        <f t="shared" ref="H39" si="9">(C39*2+F39)*0.15</f>
+        <f t="shared" ref="H39" si="10">(C39*2+F39)*0.15</f>
         <v>0</v>
       </c>
       <c r="I39" s="24"/>
@@ -3184,11 +3167,11 @@
       <c r="T39" s="24"/>
       <c r="U39" s="24"/>
       <c r="V39" s="25">
-        <f t="shared" ref="V39" si="10">(I39*0.25)+(J39*0.15)+(K39*0.1)+(L39*0.1)+(M39*0.3)+(N39*4)+(O39*4)+(IF((P39*15)&gt;40,40,(P39*15)))+(IF((Q39*2)&gt;16,16,(Q39*2)))+(R39*120)+(S39*60)+(IF((T39*3)&gt;15,15,(T39*3))+(IF((U39*6)&gt;60,60,(U39*6))))</f>
+        <f t="shared" ref="V39" si="11">(I39*0.25)+(J39*0.15)+(K39*0.1)+(L39*0.1)+(M39*0.3)+(N39*4)+(O39*4)+(IF((P39*15)&gt;40,40,(P39*15)))+(IF((Q39*2)&gt;16,16,(Q39*2)))+(R39*120)+(S39*60)+(IF((T39*3)&gt;15,15,(T39*3))+(IF((U39*6)&gt;60,60,(U39*6))))</f>
         <v>0</v>
       </c>
       <c r="W39" s="25">
-        <f t="shared" ref="W39" si="11">SUM(H39+V39)</f>
+        <f t="shared" ref="W39" si="12">SUM(H39+V39)</f>
         <v>0</v>
       </c>
       <c r="X39" s="28"/>
@@ -3293,7 +3276,10 @@
       <c r="E41" s="57"/>
       <c r="F41" s="57"/>
       <c r="G41" s="57"/>
-      <c r="H41" s="41"/>
+      <c r="H41" s="41">
+        <f t="shared" ref="H41" si="13">((IF(C41&lt;100,D41*2,D41*3)))+G41</f>
+        <v>0</v>
+      </c>
       <c r="I41" s="26"/>
       <c r="J41" s="24"/>
       <c r="K41" s="24"/>
@@ -3338,7 +3324,10 @@
       <c r="E42" s="24"/>
       <c r="F42" s="24"/>
       <c r="G42" s="30"/>
-      <c r="H42" s="41"/>
+      <c r="H42" s="41">
+        <f t="shared" ref="H42" si="14">((IF(C42&lt;100,D42*2,D42*3)))+G42</f>
+        <v>0</v>
+      </c>
       <c r="I42" s="24"/>
       <c r="J42" s="24"/>
       <c r="K42" s="24"/>
@@ -3384,7 +3373,7 @@
       <c r="F43" s="24"/>
       <c r="G43" s="31"/>
       <c r="H43" s="41">
-        <f t="shared" ref="H43:H47" si="12">((IF(C43&lt;100,IF(C43&lt;10,0.1*C43*D43*2,D43*2),D43*3)+G43*(IF(F43&lt;=10,0.1*F43,1))))</f>
+        <f t="shared" ref="H43:H47" si="15">((IF(C43&lt;100,IF(C43&lt;10,0.1*C43*D43*2,D43*2),D43*3)+G43*(IF(F43&lt;=10,0.1*F43,1))))</f>
         <v>0</v>
       </c>
       <c r="I43" s="24"/>
@@ -3401,11 +3390,11 @@
       <c r="T43" s="24"/>
       <c r="U43" s="24"/>
       <c r="V43" s="25">
-        <f t="shared" ref="V43:V47" si="13">(I43*0.25)+(J43*0.15)+(K43*0.1)+(L43*0.1)+(M43*0.3)+(N43*4)+(O43*4)+(IF((P43*15)&gt;40,40,(P43*15)))+(IF((Q43*2)&gt;16,16,(Q43*2)))+(R43*120)+(S43*60)+(IF((T43*3)&gt;15,15,(T43*3))+(IF((U43*6)&gt;60,60,(U43*6))))</f>
+        <f t="shared" ref="V43:V47" si="16">(I43*0.25)+(J43*0.15)+(K43*0.1)+(L43*0.1)+(M43*0.3)+(N43*4)+(O43*4)+(IF((P43*15)&gt;40,40,(P43*15)))+(IF((Q43*2)&gt;16,16,(Q43*2)))+(R43*120)+(S43*60)+(IF((T43*3)&gt;15,15,(T43*3))+(IF((U43*6)&gt;60,60,(U43*6))))</f>
         <v>0</v>
       </c>
       <c r="W43" s="25">
-        <f t="shared" ref="W43:W47" si="14">SUM(H43+V43)</f>
+        <f t="shared" ref="W43:W47" si="17">SUM(H43+V43)</f>
         <v>0</v>
       </c>
       <c r="X43" s="32"/>
@@ -3438,7 +3427,7 @@
       <c r="F44" s="24"/>
       <c r="G44" s="24"/>
       <c r="H44" s="41">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="I44" s="24"/>
@@ -3455,11 +3444,11 @@
       <c r="T44" s="24"/>
       <c r="U44" s="24"/>
       <c r="V44" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="W44" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="X44" s="34"/>
@@ -3492,7 +3481,7 @@
       <c r="F45" s="24"/>
       <c r="G45" s="24"/>
       <c r="H45" s="41">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="I45" s="24"/>
@@ -3509,11 +3498,11 @@
       <c r="T45" s="24"/>
       <c r="U45" s="24"/>
       <c r="V45" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="W45" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="X45" s="28"/>
@@ -3546,7 +3535,7 @@
       <c r="F46" s="24"/>
       <c r="G46" s="24"/>
       <c r="H46" s="41">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="I46" s="24"/>
@@ -3563,11 +3552,11 @@
       <c r="T46" s="24"/>
       <c r="U46" s="24"/>
       <c r="V46" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="W46" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="X46" s="28"/>
@@ -3600,7 +3589,7 @@
       <c r="F47" s="24"/>
       <c r="G47" s="24"/>
       <c r="H47" s="41">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="I47" s="24"/>
@@ -3617,11 +3606,11 @@
       <c r="T47" s="24"/>
       <c r="U47" s="24"/>
       <c r="V47" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="W47" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="X47" s="28"/>
@@ -3727,7 +3716,7 @@
       <c r="F49" s="24"/>
       <c r="G49" s="31"/>
       <c r="H49" s="41">
-        <f t="shared" ref="H49:H55" si="15">((IF(C49&lt;100,D49*2,D49*3)))+G49</f>
+        <f t="shared" ref="H49:H55" si="18">((IF(C49&lt;100,D49*2,D49*3)))+G49</f>
         <v>0</v>
       </c>
       <c r="I49" s="24"/>
@@ -3744,11 +3733,11 @@
       <c r="T49" s="24"/>
       <c r="U49" s="24"/>
       <c r="V49" s="25">
-        <f t="shared" ref="V49:V55" si="16">(I49*0.25)+(J49*0.15)+(K49*0.1)+(L49*0.1)+(M49*0.3)+(N49*4)+(O49*4)+(IF((P49*15)&gt;40,40,(P49*15)))+(IF((Q49*2)&gt;16,16,(Q49*2)))+(R49*120)+(S49*60)+(IF((T49*3)&gt;15,15,(T49*3))+(IF((U49*6)&gt;60,60,(U49*6))))</f>
+        <f t="shared" ref="V49:V55" si="19">(I49*0.25)+(J49*0.15)+(K49*0.1)+(L49*0.1)+(M49*0.3)+(N49*4)+(O49*4)+(IF((P49*15)&gt;40,40,(P49*15)))+(IF((Q49*2)&gt;16,16,(Q49*2)))+(R49*120)+(S49*60)+(IF((T49*3)&gt;15,15,(T49*3))+(IF((U49*6)&gt;60,60,(U49*6))))</f>
         <v>0</v>
       </c>
       <c r="W49" s="25">
-        <f t="shared" ref="W49:W55" si="17">SUM(H49+V49)</f>
+        <f t="shared" ref="W49:W55" si="20">SUM(H49+V49)</f>
         <v>0</v>
       </c>
       <c r="X49" s="32"/>
@@ -3781,7 +3770,7 @@
       <c r="F50" s="24"/>
       <c r="G50" s="31"/>
       <c r="H50" s="41">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="I50" s="24"/>
@@ -3798,11 +3787,11 @@
       <c r="T50" s="24"/>
       <c r="U50" s="24"/>
       <c r="V50" s="25">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="W50" s="25">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="X50" s="28"/>
@@ -3835,7 +3824,7 @@
       <c r="F51" s="24"/>
       <c r="G51" s="30"/>
       <c r="H51" s="41">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="I51" s="24"/>
@@ -3852,11 +3841,11 @@
       <c r="T51" s="24"/>
       <c r="U51" s="24"/>
       <c r="V51" s="25">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="W51" s="25">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="X51" s="4"/>
@@ -3889,7 +3878,7 @@
       <c r="F52" s="24"/>
       <c r="G52" s="30"/>
       <c r="H52" s="41">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="I52" s="24"/>
@@ -3906,11 +3895,11 @@
       <c r="T52" s="24"/>
       <c r="U52" s="24"/>
       <c r="V52" s="25">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="W52" s="25">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="X52" s="32"/>
@@ -3943,7 +3932,7 @@
       <c r="F53" s="24"/>
       <c r="G53" s="31"/>
       <c r="H53" s="41">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="I53" s="24"/>
@@ -3960,11 +3949,11 @@
       <c r="T53" s="24"/>
       <c r="U53" s="24"/>
       <c r="V53" s="25">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="W53" s="25">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="X53" s="28"/>
@@ -3997,7 +3986,7 @@
       <c r="F54" s="24"/>
       <c r="G54" s="31"/>
       <c r="H54" s="41">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="I54" s="24"/>
@@ -4014,11 +4003,11 @@
       <c r="T54" s="24"/>
       <c r="U54" s="24"/>
       <c r="V54" s="25">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="W54" s="25">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="X54" s="28"/>
@@ -4051,7 +4040,7 @@
       <c r="F55" s="24"/>
       <c r="G55" s="31"/>
       <c r="H55" s="41">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="I55" s="24"/>
@@ -4068,11 +4057,11 @@
       <c r="T55" s="24"/>
       <c r="U55" s="24"/>
       <c r="V55" s="25">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="W55" s="25">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="X55" s="28"/>
@@ -4178,7 +4167,7 @@
       <c r="F57" s="24"/>
       <c r="G57" s="31"/>
       <c r="H57" s="41">
-        <f t="shared" ref="H57:H59" si="18">(((IF(C57&lt;100,D57*2,D57*3)))+G57)*1.5</f>
+        <f t="shared" ref="H57:H59" si="21">(((IF(C57&lt;100,D57*2,D57*3)))+G57)*1.5</f>
         <v>0</v>
       </c>
       <c r="I57" s="24"/>
@@ -4195,11 +4184,11 @@
       <c r="T57" s="24"/>
       <c r="U57" s="24"/>
       <c r="V57" s="25">
-        <f t="shared" ref="V57:V59" si="19">(I57*0.25)+(J57*0.15)+(K57*0.1)+(L57*0.1)+(M57*0.3)+(N57*4)+(O57*4)+(IF((P57*15)&gt;40,40,(P57*15)))+(IF((Q57*2)&gt;16,16,(Q57*2)))+(R57*120)+(S57*60)+(IF((T57*3)&gt;15,15,(T57*3))+(IF((U57*6)&gt;60,60,(U57*6))))</f>
+        <f t="shared" ref="V57:V59" si="22">(I57*0.25)+(J57*0.15)+(K57*0.1)+(L57*0.1)+(M57*0.3)+(N57*4)+(O57*4)+(IF((P57*15)&gt;40,40,(P57*15)))+(IF((Q57*2)&gt;16,16,(Q57*2)))+(R57*120)+(S57*60)+(IF((T57*3)&gt;15,15,(T57*3))+(IF((U57*6)&gt;60,60,(U57*6))))</f>
         <v>0</v>
       </c>
       <c r="W57" s="25">
-        <f t="shared" ref="W57:W59" si="20">SUM(H57+V57)</f>
+        <f t="shared" ref="W57:W59" si="23">SUM(H57+V57)</f>
         <v>0</v>
       </c>
       <c r="X57" s="32"/>
@@ -4232,7 +4221,7 @@
       <c r="F58" s="24"/>
       <c r="G58" s="31"/>
       <c r="H58" s="41">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="I58" s="24"/>
@@ -4249,11 +4238,11 @@
       <c r="T58" s="24"/>
       <c r="U58" s="24"/>
       <c r="V58" s="25">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="W58" s="25">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="X58" s="28"/>
@@ -4286,7 +4275,7 @@
       <c r="F59" s="24"/>
       <c r="G59" s="30"/>
       <c r="H59" s="41">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="I59" s="24"/>
@@ -4303,11 +4292,11 @@
       <c r="T59" s="24"/>
       <c r="U59" s="24"/>
       <c r="V59" s="25">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="W59" s="25">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="X59" s="4"/>
@@ -4460,28 +4449,18 @@
       <c r="AQ61" s="28"/>
     </row>
     <row r="62" spans="1:43" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="58">
-        <v>26313</v>
-      </c>
-      <c r="B62" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C62" s="77">
-        <v>22</v>
-      </c>
+      <c r="A62" s="58"/>
+      <c r="B62" s="23"/>
+      <c r="C62" s="77"/>
       <c r="D62" s="60"/>
       <c r="E62" s="61"/>
-      <c r="F62" s="77">
-        <v>8</v>
-      </c>
+      <c r="F62" s="77"/>
       <c r="G62" s="61"/>
       <c r="H62" s="25">
-        <f t="shared" ref="H62:H67" si="21">(C62*2+F62)*0.15</f>
-        <v>7.8</v>
-      </c>
-      <c r="I62" s="26">
-        <v>1</v>
-      </c>
+        <f t="shared" ref="H62:H67" si="24">(C62*2+F62)*0.15</f>
+        <v>0</v>
+      </c>
+      <c r="I62" s="26"/>
       <c r="J62" s="24"/>
       <c r="K62" s="24"/>
       <c r="L62" s="24"/>
@@ -4495,12 +4474,12 @@
       <c r="T62" s="24"/>
       <c r="U62" s="24"/>
       <c r="V62" s="25">
-        <f t="shared" ref="V62:V67" si="22">(I62*0.25)+(J62*0.15)+(K62*0.1)+(L62*0.1)+(M62*0.3)+(N62*4)+(O62*4)+(IF((P62*15)&gt;40,40,(P62*15)))+(IF((Q62*2)&gt;16,16,(Q62*2)))+(R62*120)+(S62*60)+(IF((T62*3)&gt;15,15,(T62*3))+(IF((U62*6)&gt;60,60,(U62*6))))</f>
-        <v>0.25</v>
+        <f t="shared" ref="V62:V67" si="25">(I62*0.25)+(J62*0.15)+(K62*0.1)+(L62*0.1)+(M62*0.3)+(N62*4)+(O62*4)+(IF((P62*15)&gt;40,40,(P62*15)))+(IF((Q62*2)&gt;16,16,(Q62*2)))+(R62*120)+(S62*60)+(IF((T62*3)&gt;15,15,(T62*3))+(IF((U62*6)&gt;60,60,(U62*6))))</f>
+        <v>0</v>
       </c>
       <c r="W62" s="25">
-        <f t="shared" ref="W62:W67" si="23">SUM(H62+V62)</f>
-        <v>8.0500000000000007</v>
+        <f t="shared" ref="W62:W67" si="26">SUM(H62+V62)</f>
+        <v>0</v>
       </c>
       <c r="X62" s="28"/>
       <c r="Y62" s="28"/>
@@ -4532,7 +4511,7 @@
       <c r="F63" s="77"/>
       <c r="G63" s="61"/>
       <c r="H63" s="25">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="I63" s="24"/>
@@ -4549,11 +4528,11 @@
       <c r="T63" s="24"/>
       <c r="U63" s="24"/>
       <c r="V63" s="25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="W63" s="25">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="X63" s="28"/>
@@ -4586,7 +4565,7 @@
       <c r="F64" s="77"/>
       <c r="G64" s="61"/>
       <c r="H64" s="25">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="I64" s="24"/>
@@ -4603,11 +4582,11 @@
       <c r="T64" s="24"/>
       <c r="U64" s="24"/>
       <c r="V64" s="25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="W64" s="25">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="X64" s="28"/>
@@ -4640,7 +4619,7 @@
       <c r="F65" s="77"/>
       <c r="G65" s="61"/>
       <c r="H65" s="25">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="I65" s="24"/>
@@ -4657,11 +4636,11 @@
       <c r="T65" s="24"/>
       <c r="U65" s="24"/>
       <c r="V65" s="25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="W65" s="25">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="X65" s="28"/>
@@ -4694,7 +4673,7 @@
       <c r="F66" s="77"/>
       <c r="G66" s="61"/>
       <c r="H66" s="25">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="I66" s="24"/>
@@ -4711,11 +4690,11 @@
       <c r="T66" s="24"/>
       <c r="U66" s="24"/>
       <c r="V66" s="25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="W66" s="25">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="X66" s="28"/>
@@ -4748,7 +4727,7 @@
       <c r="F67" s="77"/>
       <c r="G67" s="61"/>
       <c r="H67" s="25">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="I67" s="24"/>
@@ -4765,11 +4744,11 @@
       <c r="T67" s="24"/>
       <c r="U67" s="24"/>
       <c r="V67" s="25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="W67" s="25">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="X67" s="28"/>
@@ -4801,39 +4780,39 @@
       <c r="C68" s="61"/>
       <c r="D68" s="19">
         <f>SUM(D13:D36)</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E68" s="19"/>
       <c r="F68" s="19">
         <f>SUM(F13:F36)</f>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G68" s="19">
-        <f t="shared" ref="G68:M68" si="24">SUM(G13:G39)</f>
-        <v>20</v>
+        <f t="shared" ref="G68:M68" si="27">SUM(G13:G39)</f>
+        <v>0</v>
       </c>
       <c r="H68" s="19">
-        <f t="shared" si="24"/>
-        <v>50</v>
+        <f t="shared" si="27"/>
+        <v>0</v>
       </c>
       <c r="I68" s="19">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="J68" s="19">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="K68" s="19">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="L68" s="19">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="M68" s="19">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="N68" s="19"/>
@@ -4850,7 +4829,7 @@
       </c>
       <c r="W68" s="19">
         <f>SUM(W13:W39)</f>
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="X68" s="28"/>
       <c r="Y68" s="28"/>
@@ -4885,35 +4864,35 @@
       </c>
       <c r="E69" s="43"/>
       <c r="F69" s="43">
-        <f t="shared" ref="F69:G69" si="25">SUM(F41:F59)</f>
+        <f t="shared" ref="F69:G69" si="28">SUM(F41:F59)</f>
         <v>0</v>
       </c>
       <c r="G69" s="43">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="H69" s="43">
-        <f t="shared" ref="H69:M69" si="26">SUM(H41:H67)</f>
-        <v>7.8</v>
+        <f t="shared" ref="H69:M69" si="29">SUM(H41:H67)</f>
+        <v>0</v>
       </c>
       <c r="I69" s="43">
-        <f t="shared" si="26"/>
-        <v>1</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="J69" s="43">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="K69" s="43">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="L69" s="43">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="M69" s="43">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="N69" s="43"/>
@@ -4925,12 +4904,12 @@
       <c r="T69" s="43"/>
       <c r="U69" s="43"/>
       <c r="V69" s="43">
-        <f t="shared" ref="V69:W69" si="27">SUM(V41:V67)</f>
-        <v>0.25</v>
+        <f t="shared" ref="V69:W69" si="30">SUM(V41:V67)</f>
+        <v>0</v>
       </c>
       <c r="W69" s="43">
-        <f t="shared" si="27"/>
-        <v>8.0500000000000007</v>
+        <f t="shared" si="30"/>
+        <v>0</v>
       </c>
       <c r="X69" s="28"/>
       <c r="Y69" s="28"/>
@@ -4961,80 +4940,80 @@
       <c r="C70" s="61"/>
       <c r="D70" s="22">
         <f>D68+D69</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E70" s="22"/>
       <c r="F70" s="22">
-        <f t="shared" ref="F70:M70" si="28">F68+F69</f>
-        <v>20</v>
+        <f t="shared" ref="F70:M70" si="31">F68+F69</f>
+        <v>0</v>
       </c>
       <c r="G70" s="22">
-        <f t="shared" si="28"/>
-        <v>20</v>
+        <f t="shared" si="31"/>
+        <v>0</v>
       </c>
       <c r="H70" s="22">
-        <f t="shared" si="28"/>
-        <v>57.8</v>
+        <f t="shared" si="31"/>
+        <v>0</v>
       </c>
       <c r="I70" s="22">
-        <f t="shared" si="28"/>
-        <v>1</v>
+        <f t="shared" si="31"/>
+        <v>0</v>
       </c>
       <c r="J70" s="22">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="K70" s="22">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="L70" s="22">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="M70" s="22">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="N70" s="22">
-        <f t="shared" ref="N70:U70" si="29">SUM(N13:N67)</f>
+        <f t="shared" ref="N70:U70" si="32">SUM(N13:N67)</f>
         <v>0</v>
       </c>
       <c r="O70" s="22">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="P70" s="22">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="Q70" s="22">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="R70" s="22">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="S70" s="22">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="T70" s="22">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="U70" s="22">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="V70" s="22">
-        <f t="shared" ref="V70:W70" si="30">V68+V69</f>
-        <v>0.25</v>
+        <f t="shared" ref="V70:W70" si="33">V68+V69</f>
+        <v>0</v>
       </c>
       <c r="W70" s="22">
-        <f t="shared" si="30"/>
-        <v>58.05</v>
+        <f t="shared" si="33"/>
+        <v>0</v>
       </c>
       <c r="X70" s="28"/>
       <c r="Y70" s="28"/>
@@ -5280,7 +5259,7 @@
       <c r="V75" s="4"/>
       <c r="W75" s="46">
         <f>IF((H70+W71+W72)&gt;=W8,(H70+W71+W72-W8)+V70+W73,0)</f>
-        <v>58.05</v>
+        <v>0</v>
       </c>
       <c r="X75" s="1"/>
       <c r="Y75" s="1"/>
@@ -5330,7 +5309,7 @@
       <c r="V76" s="4"/>
       <c r="W76" s="46">
         <f>IF((H68+W71)&lt;=840,W75-W74,(W75-(H68+W71-840)-W74))</f>
-        <v>58.05</v>
+        <v>0</v>
       </c>
       <c r="X76" s="1"/>
       <c r="Y76" s="1"/>

</xml_diff>